<commit_message>
Added codebook field descriptions pickles
</commit_message>
<xml_diff>
--- a/metadata/FieldDescriptions.xlsx
+++ b/metadata/FieldDescriptions.xlsx
@@ -8,12 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/98c3d89177ee1291/Documents/GitHub/CaLPA/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="235" documentId="8_{C02E4E36-9E37-448D-B4AD-D3D7E3C757E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C77FBCD-FFA5-4A3A-AFA2-B3C81EB34FE2}"/>
+  <xr:revisionPtr revIDLastSave="667" documentId="8_{C02E4E36-9E37-448D-B4AD-D3D7E3C757E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E13DF9B8-F1BD-4FE5-9999-9BEC0B195ECF}"/>
   <bookViews>
-    <workbookView xWindow="7000" yWindow="9840" windowWidth="16740" windowHeight="6160" xr2:uid="{575AF95D-8A6E-4F2F-A913-B968B52F4ECB}"/>
+    <workbookView xWindow="7000" yWindow="9760" windowWidth="16740" windowHeight="6160" firstSheet="3" activeTab="6" xr2:uid="{575AF95D-8A6E-4F2F-A913-B968B52F4ECB}"/>
   </bookViews>
   <sheets>
     <sheet name="getBill" sheetId="1" r:id="rId1"/>
+    <sheet name="getRollCall" sheetId="2" r:id="rId2"/>
+    <sheet name="getBillText" sheetId="3" r:id="rId3"/>
+    <sheet name="getAmendment" sheetId="4" r:id="rId4"/>
+    <sheet name="getSupplement" sheetId="5" r:id="rId5"/>
+    <sheet name="getPerson" sheetId="6" r:id="rId6"/>
+    <sheet name="getSessionList" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="290">
   <si>
     <t>Field</t>
   </si>
@@ -822,6 +828,90 @@
   </si>
   <si>
     <t>Event description</t>
+  </si>
+  <si>
+    <t>Vote date (if available)</t>
+  </si>
+  <si>
+    <t>Vote description</t>
+  </si>
+  <si>
+    <t>Array of vote details</t>
+  </si>
+  <si>
+    <t>Individual vote record</t>
+  </si>
+  <si>
+    <t>vote_id</t>
+  </si>
+  <si>
+    <t>Internal vote type ID</t>
+  </si>
+  <si>
+    <t>vote_text</t>
+  </si>
+  <si>
+    <t>Vote type ID description text (Yea, Nay, NV, Absent)</t>
+  </si>
+  <si>
+    <t>Internal document ID</t>
+  </si>
+  <si>
+    <t>Document date (if available)</t>
+  </si>
+  <si>
+    <t>Type of draft text</t>
+  </si>
+  <si>
+    <t>Internal text type ID</t>
+  </si>
+  <si>
+    <t>doc</t>
+  </si>
+  <si>
+    <t>BASE64 encoded document</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>Chamber of origin</t>
+  </si>
+  <si>
+    <t>Amendment description</t>
+  </si>
+  <si>
+    <t>Type of supplement</t>
+  </si>
+  <si>
+    <t>Party text (D, R, I, etc)</t>
+  </si>
+  <si>
+    <t>Role text (Rep, Sen, etc)</t>
+  </si>
+  <si>
+    <t>ftm_eid</t>
+  </si>
+  <si>
+    <t>FollowTheMoney.org EID</t>
+  </si>
+  <si>
+    <t>Starting year of session</t>
+  </si>
+  <si>
+    <t>Ending year of session</t>
+  </si>
+  <si>
+    <t>prefile</t>
+  </si>
+  <si>
+    <t>Flag for session being archived (0, 1)</t>
+  </si>
+  <si>
+    <t>Flag for session being adjourned sine die (0, 1)</t>
+  </si>
+  <si>
+    <t>Normalized session title with year(s) and Regular/Nth Special Session</t>
   </si>
 </sst>
 </file>
@@ -874,6 +964,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1195,15 +1289,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED06A460-9FDE-4F8B-803B-BA3A3A775BDD}">
   <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1231,6 +1324,9 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
@@ -1245,6 +1341,9 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
+      <c r="C3" t="s">
+        <v>276</v>
+      </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
@@ -1259,6 +1358,9 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
+      <c r="C4" t="s">
+        <v>276</v>
+      </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
@@ -1272,6 +1374,9 @@
       </c>
       <c r="B5" t="s">
         <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>276</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -1287,6 +1392,9 @@
       <c r="B6" t="s">
         <v>15</v>
       </c>
+      <c r="C6" t="s">
+        <v>276</v>
+      </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
@@ -1301,6 +1409,9 @@
       <c r="B7" t="s">
         <v>17</v>
       </c>
+      <c r="C7" t="s">
+        <v>276</v>
+      </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
@@ -1468,6 +1579,9 @@
       <c r="B17" t="s">
         <v>21</v>
       </c>
+      <c r="C17" t="s">
+        <v>276</v>
+      </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
@@ -1482,6 +1596,9 @@
       <c r="B18" t="s">
         <v>48</v>
       </c>
+      <c r="C18" t="s">
+        <v>276</v>
+      </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
@@ -1496,6 +1613,9 @@
       <c r="B19" t="s">
         <v>22</v>
       </c>
+      <c r="C19" t="s">
+        <v>276</v>
+      </c>
       <c r="D19" t="s">
         <v>4</v>
       </c>
@@ -1510,6 +1630,9 @@
       <c r="B20" t="s">
         <v>51</v>
       </c>
+      <c r="C20" t="s">
+        <v>276</v>
+      </c>
       <c r="D20" t="s">
         <v>4</v>
       </c>
@@ -1524,6 +1647,9 @@
       <c r="B21" t="s">
         <v>23</v>
       </c>
+      <c r="C21" t="s">
+        <v>276</v>
+      </c>
       <c r="D21" t="s">
         <v>24</v>
       </c>
@@ -1538,6 +1664,9 @@
       <c r="B22" t="s">
         <v>54</v>
       </c>
+      <c r="C22" t="s">
+        <v>276</v>
+      </c>
       <c r="D22" t="s">
         <v>13</v>
       </c>
@@ -1603,6 +1732,9 @@
       <c r="B26" t="s">
         <v>61</v>
       </c>
+      <c r="C26" t="s">
+        <v>276</v>
+      </c>
       <c r="D26" t="s">
         <v>7</v>
       </c>
@@ -1617,6 +1749,9 @@
       <c r="B27" t="s">
         <v>27</v>
       </c>
+      <c r="C27" t="s">
+        <v>276</v>
+      </c>
       <c r="D27" t="s">
         <v>4</v>
       </c>
@@ -1631,6 +1766,9 @@
       <c r="B28" t="s">
         <v>64</v>
       </c>
+      <c r="C28" t="s">
+        <v>276</v>
+      </c>
       <c r="D28" t="s">
         <v>7</v>
       </c>
@@ -1645,6 +1783,9 @@
       <c r="B29" t="s">
         <v>28</v>
       </c>
+      <c r="C29" t="s">
+        <v>276</v>
+      </c>
       <c r="D29" t="s">
         <v>7</v>
       </c>
@@ -1659,6 +1800,9 @@
       <c r="B30" t="s">
         <v>67</v>
       </c>
+      <c r="C30" t="s">
+        <v>276</v>
+      </c>
       <c r="D30" t="s">
         <v>4</v>
       </c>
@@ -1673,6 +1817,9 @@
       <c r="B31" t="s">
         <v>29</v>
       </c>
+      <c r="C31" t="s">
+        <v>276</v>
+      </c>
       <c r="D31" t="s">
         <v>7</v>
       </c>
@@ -1687,6 +1834,9 @@
       <c r="B32" t="s">
         <v>70</v>
       </c>
+      <c r="C32" t="s">
+        <v>276</v>
+      </c>
       <c r="D32" t="s">
         <v>4</v>
       </c>
@@ -1701,6 +1851,9 @@
       <c r="B33" t="s">
         <v>30</v>
       </c>
+      <c r="C33" t="s">
+        <v>276</v>
+      </c>
       <c r="D33" t="s">
         <v>7</v>
       </c>
@@ -1715,6 +1868,9 @@
       <c r="B34" t="s">
         <v>73</v>
       </c>
+      <c r="C34" t="s">
+        <v>276</v>
+      </c>
       <c r="D34" t="s">
         <v>4</v>
       </c>
@@ -1729,6 +1885,9 @@
       <c r="B35" t="s">
         <v>74</v>
       </c>
+      <c r="C35" t="s">
+        <v>276</v>
+      </c>
       <c r="D35" t="s">
         <v>7</v>
       </c>
@@ -1743,6 +1902,9 @@
       <c r="B36" t="s">
         <v>76</v>
       </c>
+      <c r="C36" t="s">
+        <v>276</v>
+      </c>
       <c r="D36" t="s">
         <v>7</v>
       </c>
@@ -1757,6 +1919,9 @@
       <c r="B37" t="s">
         <v>77</v>
       </c>
+      <c r="C37" t="s">
+        <v>276</v>
+      </c>
       <c r="D37" t="s">
         <v>4</v>
       </c>
@@ -1771,6 +1936,9 @@
       <c r="B38" t="s">
         <v>79</v>
       </c>
+      <c r="C38" t="s">
+        <v>276</v>
+      </c>
       <c r="D38" t="s">
         <v>13</v>
       </c>
@@ -1853,6 +2021,9 @@
       <c r="B43" t="s">
         <v>88</v>
       </c>
+      <c r="C43" t="s">
+        <v>276</v>
+      </c>
       <c r="D43" t="s">
         <v>13</v>
       </c>
@@ -1969,6 +2140,9 @@
       <c r="B50" t="s">
         <v>95</v>
       </c>
+      <c r="C50" t="s">
+        <v>276</v>
+      </c>
       <c r="D50" t="s">
         <v>13</v>
       </c>
@@ -2011,6 +2185,9 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>52</v>
+      </c>
       <c r="B53" t="s">
         <v>99</v>
       </c>
@@ -2025,6 +2202,9 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>53</v>
+      </c>
       <c r="B54" t="s">
         <v>83</v>
       </c>
@@ -2039,6 +2219,9 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>54</v>
+      </c>
       <c r="B55" t="s">
         <v>85</v>
       </c>
@@ -2053,6 +2236,9 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>55</v>
+      </c>
       <c r="B56" t="s">
         <v>102</v>
       </c>
@@ -2067,9 +2253,15 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>56</v>
+      </c>
       <c r="B57" t="s">
         <v>105</v>
       </c>
+      <c r="C57" t="s">
+        <v>276</v>
+      </c>
       <c r="D57" t="s">
         <v>13</v>
       </c>
@@ -2078,6 +2270,9 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>57</v>
+      </c>
       <c r="B58" t="s">
         <v>107</v>
       </c>
@@ -2092,6 +2287,9 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>58</v>
+      </c>
       <c r="B59" t="s">
         <v>110</v>
       </c>
@@ -2106,6 +2304,9 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>59</v>
+      </c>
       <c r="B60" t="s">
         <v>113</v>
       </c>
@@ -2120,6 +2321,9 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>60</v>
+      </c>
       <c r="B61" t="s">
         <v>115</v>
       </c>
@@ -2134,6 +2338,9 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>61</v>
+      </c>
       <c r="B62" t="s">
         <v>118</v>
       </c>
@@ -2148,6 +2355,9 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>62</v>
+      </c>
       <c r="B63" t="s">
         <v>119</v>
       </c>
@@ -2162,6 +2372,9 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>63</v>
+      </c>
       <c r="B64" t="s">
         <v>121</v>
       </c>
@@ -2175,7 +2388,10 @@
         <v>122</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>64</v>
+      </c>
       <c r="B65" t="s">
         <v>123</v>
       </c>
@@ -2189,7 +2405,10 @@
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>65</v>
+      </c>
       <c r="B66" t="s">
         <v>125</v>
       </c>
@@ -2203,7 +2422,10 @@
         <v>126</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>66</v>
+      </c>
       <c r="B67" t="s">
         <v>127</v>
       </c>
@@ -2217,7 +2439,10 @@
         <v>128</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>67</v>
+      </c>
       <c r="B68" t="s">
         <v>129</v>
       </c>
@@ -2231,7 +2456,10 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>68</v>
+      </c>
       <c r="B69" t="s">
         <v>131</v>
       </c>
@@ -2245,7 +2473,10 @@
         <v>132</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>69</v>
+      </c>
       <c r="B70" t="s">
         <v>133</v>
       </c>
@@ -2259,7 +2490,10 @@
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>70</v>
+      </c>
       <c r="B71" t="s">
         <v>135</v>
       </c>
@@ -2273,7 +2507,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>71</v>
+      </c>
       <c r="B72" t="s">
         <v>137</v>
       </c>
@@ -2287,7 +2524,10 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>72</v>
+      </c>
       <c r="B73" t="s">
         <v>139</v>
       </c>
@@ -2301,7 +2541,10 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>73</v>
+      </c>
       <c r="B74" t="s">
         <v>141</v>
       </c>
@@ -2315,7 +2558,10 @@
         <v>142</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>74</v>
+      </c>
       <c r="B75" t="s">
         <v>143</v>
       </c>
@@ -2329,7 +2575,10 @@
         <v>144</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>75</v>
+      </c>
       <c r="B76" t="s">
         <v>146</v>
       </c>
@@ -2343,7 +2592,10 @@
         <v>145</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>76</v>
+      </c>
       <c r="B77" t="s">
         <v>147</v>
       </c>
@@ -2357,7 +2609,10 @@
         <v>148</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>77</v>
+      </c>
       <c r="B78" t="s">
         <v>81</v>
       </c>
@@ -2371,10 +2626,16 @@
         <v>149</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>78</v>
+      </c>
       <c r="B79" t="s">
         <v>150</v>
       </c>
+      <c r="C79" t="s">
+        <v>276</v>
+      </c>
       <c r="D79" t="s">
         <v>13</v>
       </c>
@@ -2382,7 +2643,10 @@
         <v>151</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>79</v>
+      </c>
       <c r="B80" t="s">
         <v>152</v>
       </c>
@@ -2396,7 +2660,10 @@
         <v>154</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>80</v>
+      </c>
       <c r="B81" t="s">
         <v>155</v>
       </c>
@@ -2410,7 +2677,10 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>81</v>
+      </c>
       <c r="B82" t="s">
         <v>158</v>
       </c>
@@ -2424,7 +2694,10 @@
         <v>159</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>82</v>
+      </c>
       <c r="B83" t="s">
         <v>160</v>
       </c>
@@ -2438,7 +2711,10 @@
         <v>161</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>83</v>
+      </c>
       <c r="B84" t="s">
         <v>162</v>
       </c>
@@ -2452,10 +2728,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>84</v>
+      </c>
       <c r="B85" t="s">
         <v>163</v>
       </c>
+      <c r="C85" t="s">
+        <v>276</v>
+      </c>
       <c r="D85" t="s">
         <v>13</v>
       </c>
@@ -2463,7 +2745,10 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>85</v>
+      </c>
       <c r="B86" t="s">
         <v>165</v>
       </c>
@@ -2477,7 +2762,10 @@
         <v>167</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>86</v>
+      </c>
       <c r="B87" t="s">
         <v>168</v>
       </c>
@@ -2491,7 +2779,10 @@
         <v>170</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>87</v>
+      </c>
       <c r="B88" t="s">
         <v>171</v>
       </c>
@@ -2505,10 +2796,16 @@
         <v>172</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>88</v>
+      </c>
       <c r="B89" t="s">
         <v>173</v>
       </c>
+      <c r="C89" t="s">
+        <v>276</v>
+      </c>
       <c r="D89" t="s">
         <v>13</v>
       </c>
@@ -2516,7 +2813,10 @@
         <v>174</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>89</v>
+      </c>
       <c r="B90" t="s">
         <v>175</v>
       </c>
@@ -2530,7 +2830,10 @@
         <v>177</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>90</v>
+      </c>
       <c r="B91" t="s">
         <v>178</v>
       </c>
@@ -2544,7 +2847,10 @@
         <v>180</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>91</v>
+      </c>
       <c r="B92" t="s">
         <v>24</v>
       </c>
@@ -2558,7 +2864,10 @@
         <v>181</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>92</v>
+      </c>
       <c r="B93" t="s">
         <v>158</v>
       </c>
@@ -2572,7 +2881,10 @@
         <v>182</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>93</v>
+      </c>
       <c r="B94" t="s">
         <v>155</v>
       </c>
@@ -2586,7 +2898,10 @@
         <v>183</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>94</v>
+      </c>
       <c r="B95" t="s">
         <v>184</v>
       </c>
@@ -2600,7 +2915,10 @@
         <v>185</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>95</v>
+      </c>
       <c r="B96" t="s">
         <v>186</v>
       </c>
@@ -2614,7 +2932,10 @@
         <v>187</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>96</v>
+      </c>
       <c r="B97" t="s">
         <v>21</v>
       </c>
@@ -2628,7 +2949,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>97</v>
+      </c>
       <c r="B98" t="s">
         <v>48</v>
       </c>
@@ -2642,7 +2966,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>98</v>
+      </c>
       <c r="B99" t="s">
         <v>188</v>
       </c>
@@ -2656,7 +2983,10 @@
         <v>189</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>99</v>
+      </c>
       <c r="B100" t="s">
         <v>190</v>
       </c>
@@ -2670,10 +3000,16 @@
         <v>191</v>
       </c>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>100</v>
+      </c>
       <c r="B101" t="s">
         <v>192</v>
       </c>
+      <c r="C101" t="s">
+        <v>276</v>
+      </c>
       <c r="D101" t="s">
         <v>13</v>
       </c>
@@ -2681,7 +3017,10 @@
         <v>193</v>
       </c>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>101</v>
+      </c>
       <c r="B102" t="s">
         <v>194</v>
       </c>
@@ -2695,7 +3034,10 @@
         <v>196</v>
       </c>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>102</v>
+      </c>
       <c r="B103" t="s">
         <v>197</v>
       </c>
@@ -2709,7 +3051,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>103</v>
+      </c>
       <c r="B104" t="s">
         <v>24</v>
       </c>
@@ -2723,7 +3068,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>104</v>
+      </c>
       <c r="B105" t="s">
         <v>201</v>
       </c>
@@ -2737,7 +3085,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>105</v>
+      </c>
       <c r="B106" t="s">
         <v>203</v>
       </c>
@@ -2751,7 +3102,10 @@
         <v>204</v>
       </c>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>106</v>
+      </c>
       <c r="B107" t="s">
         <v>205</v>
       </c>
@@ -2765,7 +3119,10 @@
         <v>206</v>
       </c>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>107</v>
+      </c>
       <c r="B108" t="s">
         <v>207</v>
       </c>
@@ -2779,7 +3136,10 @@
         <v>208</v>
       </c>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>108</v>
+      </c>
       <c r="B109" t="s">
         <v>209</v>
       </c>
@@ -2793,7 +3153,10 @@
         <v>210</v>
       </c>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>109</v>
+      </c>
       <c r="B110" t="s">
         <v>211</v>
       </c>
@@ -2807,7 +3170,10 @@
         <v>212</v>
       </c>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>110</v>
+      </c>
       <c r="B111" t="s">
         <v>213</v>
       </c>
@@ -2821,7 +3187,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>111</v>
+      </c>
       <c r="B112" t="s">
         <v>83</v>
       </c>
@@ -2835,7 +3204,10 @@
         <v>215</v>
       </c>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>112</v>
+      </c>
       <c r="B113" t="s">
         <v>85</v>
       </c>
@@ -2849,7 +3221,10 @@
         <v>216</v>
       </c>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>113</v>
+      </c>
       <c r="B114" t="s">
         <v>21</v>
       </c>
@@ -2863,7 +3238,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>114</v>
+      </c>
       <c r="B115" t="s">
         <v>48</v>
       </c>
@@ -2877,10 +3255,16 @@
         <v>49</v>
       </c>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>115</v>
+      </c>
       <c r="B116" t="s">
         <v>217</v>
       </c>
+      <c r="C116" t="s">
+        <v>276</v>
+      </c>
       <c r="D116" t="s">
         <v>13</v>
       </c>
@@ -2888,7 +3272,10 @@
         <v>218</v>
       </c>
     </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>116</v>
+      </c>
       <c r="B117" t="s">
         <v>219</v>
       </c>
@@ -2902,7 +3289,10 @@
         <v>221</v>
       </c>
     </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>117</v>
+      </c>
       <c r="B118" t="s">
         <v>222</v>
       </c>
@@ -2916,7 +3306,10 @@
         <v>224</v>
       </c>
     </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>118</v>
+      </c>
       <c r="B119" t="s">
         <v>225</v>
       </c>
@@ -2930,7 +3323,10 @@
         <v>226</v>
       </c>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A120">
+        <v>119</v>
+      </c>
       <c r="B120" t="s">
         <v>83</v>
       </c>
@@ -2944,7 +3340,10 @@
         <v>227</v>
       </c>
     </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A121">
+        <v>120</v>
+      </c>
       <c r="B121" t="s">
         <v>85</v>
       </c>
@@ -2958,7 +3357,10 @@
         <v>71</v>
       </c>
     </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <v>121</v>
+      </c>
       <c r="B122" t="s">
         <v>24</v>
       </c>
@@ -2972,7 +3374,10 @@
         <v>228</v>
       </c>
     </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A123">
+        <v>122</v>
+      </c>
       <c r="B123" t="s">
         <v>74</v>
       </c>
@@ -2986,7 +3391,10 @@
         <v>229</v>
       </c>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A124">
+        <v>123</v>
+      </c>
       <c r="B124" t="s">
         <v>76</v>
       </c>
@@ -3000,7 +3408,10 @@
         <v>230</v>
       </c>
     </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A125">
+        <v>124</v>
+      </c>
       <c r="B125" t="s">
         <v>184</v>
       </c>
@@ -3014,7 +3425,10 @@
         <v>185</v>
       </c>
     </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <v>125</v>
+      </c>
       <c r="B126" t="s">
         <v>186</v>
       </c>
@@ -3028,7 +3442,10 @@
         <v>231</v>
       </c>
     </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A127">
+        <v>126</v>
+      </c>
       <c r="B127" t="s">
         <v>21</v>
       </c>
@@ -3042,7 +3459,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>127</v>
+      </c>
       <c r="B128" t="s">
         <v>48</v>
       </c>
@@ -3056,7 +3476,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <v>128</v>
+      </c>
       <c r="B129" t="s">
         <v>232</v>
       </c>
@@ -3070,7 +3493,10 @@
         <v>189</v>
       </c>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A130">
+        <v>129</v>
+      </c>
       <c r="B130" t="s">
         <v>233</v>
       </c>
@@ -3084,10 +3510,16 @@
         <v>191</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A131">
+        <v>130</v>
+      </c>
       <c r="B131" t="s">
         <v>234</v>
       </c>
+      <c r="C131" t="s">
+        <v>276</v>
+      </c>
       <c r="D131" t="s">
         <v>13</v>
       </c>
@@ -3095,7 +3527,10 @@
         <v>235</v>
       </c>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A132">
+        <v>131</v>
+      </c>
       <c r="B132" t="s">
         <v>236</v>
       </c>
@@ -3109,7 +3544,10 @@
         <v>238</v>
       </c>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A133">
+        <v>132</v>
+      </c>
       <c r="B133" t="s">
         <v>239</v>
       </c>
@@ -3123,7 +3561,10 @@
         <v>241</v>
       </c>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A134">
+        <v>133</v>
+      </c>
       <c r="B134" t="s">
         <v>24</v>
       </c>
@@ -3137,7 +3578,10 @@
         <v>242</v>
       </c>
     </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <v>134</v>
+      </c>
       <c r="B135" t="s">
         <v>155</v>
       </c>
@@ -3151,7 +3595,10 @@
         <v>243</v>
       </c>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <v>135</v>
+      </c>
       <c r="B136" t="s">
         <v>158</v>
       </c>
@@ -3165,7 +3612,10 @@
         <v>244</v>
       </c>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <v>136</v>
+      </c>
       <c r="B137" t="s">
         <v>74</v>
       </c>
@@ -3179,7 +3629,10 @@
         <v>245</v>
       </c>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A138">
+        <v>137</v>
+      </c>
       <c r="B138" t="s">
         <v>76</v>
       </c>
@@ -3193,7 +3646,10 @@
         <v>246</v>
       </c>
     </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A139">
+        <v>138</v>
+      </c>
       <c r="B139" t="s">
         <v>184</v>
       </c>
@@ -3207,7 +3663,10 @@
         <v>185</v>
       </c>
     </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A140">
+        <v>139</v>
+      </c>
       <c r="B140" t="s">
         <v>186</v>
       </c>
@@ -3221,7 +3680,10 @@
         <v>187</v>
       </c>
     </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A141">
+        <v>140</v>
+      </c>
       <c r="B141" t="s">
         <v>21</v>
       </c>
@@ -3235,7 +3697,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <v>141</v>
+      </c>
       <c r="B142" t="s">
         <v>48</v>
       </c>
@@ -3249,7 +3714,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A143">
+        <v>142</v>
+      </c>
       <c r="B143" t="s">
         <v>247</v>
       </c>
@@ -3263,7 +3731,10 @@
         <v>189</v>
       </c>
     </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A144">
+        <v>143</v>
+      </c>
       <c r="B144" t="s">
         <v>248</v>
       </c>
@@ -3277,10 +3748,16 @@
         <v>191</v>
       </c>
     </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A145">
+        <v>144</v>
+      </c>
       <c r="B145" t="s">
         <v>249</v>
       </c>
+      <c r="C145" t="s">
+        <v>276</v>
+      </c>
       <c r="D145" t="s">
         <v>13</v>
       </c>
@@ -3288,7 +3765,10 @@
         <v>250</v>
       </c>
     </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <v>145</v>
+      </c>
       <c r="B146" t="s">
         <v>251</v>
       </c>
@@ -3302,7 +3782,10 @@
         <v>253</v>
       </c>
     </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <v>146</v>
+      </c>
       <c r="B147" t="s">
         <v>155</v>
       </c>
@@ -3316,7 +3799,10 @@
         <v>254</v>
       </c>
     </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <v>147</v>
+      </c>
       <c r="B148" t="s">
         <v>158</v>
       </c>
@@ -3330,7 +3816,10 @@
         <v>255</v>
       </c>
     </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A149">
+        <v>148</v>
+      </c>
       <c r="B149" t="s">
         <v>24</v>
       </c>
@@ -3344,7 +3833,10 @@
         <v>256</v>
       </c>
     </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>149</v>
+      </c>
       <c r="B150" t="s">
         <v>257</v>
       </c>
@@ -3358,7 +3850,10 @@
         <v>258</v>
       </c>
     </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>150</v>
+      </c>
       <c r="B151" t="s">
         <v>259</v>
       </c>
@@ -3372,7 +3867,10 @@
         <v>260</v>
       </c>
     </row>
-    <row r="152" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>151</v>
+      </c>
       <c r="B152" t="s">
         <v>76</v>
       </c>
@@ -3384,6 +3882,1634 @@
       </c>
       <c r="E152" t="s">
         <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A1654C-D808-4F0D-B7F4-16FB7C115F13}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C10" t="s">
+        <v>276</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C11" t="s">
+        <v>276</v>
+      </c>
+      <c r="D11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>276</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" t="s">
+        <v>276</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C14" t="s">
+        <v>276</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15" t="s">
+        <v>195</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" t="s">
+        <v>198</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>266</v>
+      </c>
+      <c r="C17" t="s">
+        <v>198</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>268</v>
+      </c>
+      <c r="C18" t="s">
+        <v>198</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01306E15-C62A-4C07-9155-19543F7DDB3A}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" t="s">
+        <v>276</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>274</v>
+      </c>
+      <c r="C11" t="s">
+        <v>276</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067E4D68-471F-4DF6-A25A-C8A6DDF576ED}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" t="s">
+        <v>276</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C11" t="s">
+        <v>276</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>232</v>
+      </c>
+      <c r="C12" t="s">
+        <v>276</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C13" t="s">
+        <v>276</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" t="s">
+        <v>276</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C5A6B66-8341-4819-9892-12D868F9DF95}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C10" t="s">
+        <v>276</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" t="s">
+        <v>276</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>248</v>
+      </c>
+      <c r="C12" t="s">
+        <v>276</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>274</v>
+      </c>
+      <c r="C13" t="s">
+        <v>276</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61DB3AF-4DA7-4EF1-B1F8-CCB9E82450A4}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" t="s">
+        <v>276</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" t="s">
+        <v>276</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" t="s">
+        <v>276</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" t="s">
+        <v>276</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" t="s">
+        <v>276</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>282</v>
+      </c>
+      <c r="C15" t="s">
+        <v>276</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" t="s">
+        <v>276</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" t="s">
+        <v>276</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" t="s">
+        <v>276</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" t="s">
+        <v>276</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" t="s">
+        <v>276</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>276</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719F4A42-95FE-4519-84A8-9C8E20925524}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>276</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>276</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add AI notes for various bills and resolutions for the 2023-2024 and 2025-2026 sessions
</commit_message>
<xml_diff>
--- a/metadata/FieldDescriptions.xlsx
+++ b/metadata/FieldDescriptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/98c3d89177ee1291/Documents/GitHub/CaLPA/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="667" documentId="8_{C02E4E36-9E37-448D-B4AD-D3D7E3C757E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E13DF9B8-F1BD-4FE5-9999-9BEC0B195ECF}"/>
+  <xr:revisionPtr revIDLastSave="674" documentId="8_{C02E4E36-9E37-448D-B4AD-D3D7E3C757E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49B6B124-F180-406C-B17E-07438FD5384A}"/>
   <bookViews>
-    <workbookView xWindow="7000" yWindow="9760" windowWidth="16740" windowHeight="6160" firstSheet="3" activeTab="6" xr2:uid="{575AF95D-8A6E-4F2F-A913-B968B52F4ECB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{575AF95D-8A6E-4F2F-A913-B968B52F4ECB}"/>
   </bookViews>
   <sheets>
     <sheet name="getBill" sheetId="1" r:id="rId1"/>
@@ -968,6 +968,20 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{658C84AD-A0D4-4F0F-AF02-8DA844C8512D}" name="Table1" displayName="Table1" ref="A1:E152" totalsRowShown="0">
+  <autoFilter ref="A1:E152" xr:uid="{658C84AD-A0D4-4F0F-AF02-8DA844C8512D}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{0A5CF1D5-B100-4579-8A65-A59C30E675FC}" name="Order"/>
+    <tableColumn id="2" xr3:uid="{C46AA331-8D6F-4D53-A080-E31D50EDC589}" name="Field"/>
+    <tableColumn id="3" xr3:uid="{7CFA4213-992B-43A1-91B1-1CFC0D6A4FC8}" name="Parent"/>
+    <tableColumn id="4" xr3:uid="{2221CE23-9243-4F59-B2EC-14B7200CD389}" name="Type"/>
+    <tableColumn id="5" xr3:uid="{2560F5F1-389A-4E5C-9243-BED53096A52B}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1289,11 +1303,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED06A460-9FDE-4F8B-803B-BA3A3A775BDD}">
   <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.453125" customWidth="1"/>
     <col min="2" max="2" width="19.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.08984375" bestFit="1" customWidth="1"/>
@@ -3886,6 +3902,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -5312,7 +5331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719F4A42-95FE-4519-84A8-9C8E20925524}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Restructured calpa package and modules and rerun the code
</commit_message>
<xml_diff>
--- a/metadata/FieldDescriptions.xlsx
+++ b/metadata/FieldDescriptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/98c3d89177ee1291/Documents/GitHub/CaLPA/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="674" documentId="8_{C02E4E36-9E37-448D-B4AD-D3D7E3C757E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49B6B124-F180-406C-B17E-07438FD5384A}"/>
+  <xr:revisionPtr revIDLastSave="676" documentId="8_{C02E4E36-9E37-448D-B4AD-D3D7E3C757E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC8B3AA6-96C3-472D-B33A-9F77B320754B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{575AF95D-8A6E-4F2F-A913-B968B52F4ECB}"/>
+    <workbookView xWindow="12490" yWindow="0" windowWidth="12560" windowHeight="16010" firstSheet="3" activeTab="3" xr2:uid="{575AF95D-8A6E-4F2F-A913-B968B52F4ECB}"/>
   </bookViews>
   <sheets>
     <sheet name="getBill" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="291">
   <si>
     <t>Field</t>
   </si>
@@ -912,6 +912,9 @@
   </si>
   <si>
     <t>Normalized session title with year(s) and Regular/Nth Special Session</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -1303,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED06A460-9FDE-4F8B-803B-BA3A3A775BDD}">
   <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A127" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1313,7 +1316,7 @@
     <col min="2" max="2" width="19.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -3902,8 +3905,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3913,7 +3917,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4414,7 +4418,7 @@
         <v>190</v>
       </c>
       <c r="C10" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -4449,7 +4453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067E4D68-471F-4DF6-A25A-C8A6DDF576ED}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>